<commit_message>
first successful regression replicate
</commit_message>
<xml_diff>
--- a/data/FOMC_Cycle_dates_2010_2016.xlsx
+++ b/data/FOMC_Cycle_dates_2010_2016.xlsx
@@ -275,13 +275,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F68"/>
+  <dimension ref="A1:F92"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.15"/>
@@ -811,6 +811,184 @@
       </c>
       <c r="B68" s="4" t="n">
         <v>40205</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="4" t="n">
+        <v>40162</v>
+      </c>
+      <c r="B69" s="4" t="n">
+        <v>40163</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="4" t="n">
+        <v>40120</v>
+      </c>
+      <c r="B70" s="4" t="n">
+        <v>40121</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="4" t="n">
+        <v>40078</v>
+      </c>
+      <c r="B71" s="4" t="n">
+        <v>40079</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="4" t="n">
+        <v>40036</v>
+      </c>
+      <c r="B72" s="4" t="n">
+        <v>40037</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="4" t="n">
+        <v>39987</v>
+      </c>
+      <c r="B73" s="4" t="n">
+        <v>39988</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="4" t="n">
+        <v>39931</v>
+      </c>
+      <c r="B74" s="4" t="n">
+        <v>39932</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="4" t="n">
+        <v>39889</v>
+      </c>
+      <c r="B75" s="4" t="n">
+        <v>39890</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="4" t="n">
+        <v>39840</v>
+      </c>
+      <c r="B76" s="4" t="n">
+        <v>39841</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="4" t="n">
+        <v>39797</v>
+      </c>
+      <c r="B77" s="4" t="n">
+        <v>39798</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="4" t="n">
+        <v>39749</v>
+      </c>
+      <c r="B78" s="4" t="n">
+        <v>39750</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="4" t="n">
+        <v>39707</v>
+      </c>
+      <c r="B79" s="4"/>
+    </row>
+    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="4" t="n">
+        <v>39665</v>
+      </c>
+      <c r="B80" s="4"/>
+    </row>
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="4" t="n">
+        <v>39623</v>
+      </c>
+      <c r="B81" s="4" t="n">
+        <v>39624</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="4" t="n">
+        <v>39567</v>
+      </c>
+      <c r="B82" s="4" t="n">
+        <v>39568</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="4" t="n">
+        <v>39525</v>
+      </c>
+      <c r="B83" s="4"/>
+    </row>
+    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="4" t="n">
+        <v>39476</v>
+      </c>
+      <c r="B84" s="4" t="n">
+        <v>39477</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="4" t="n">
+        <v>39427</v>
+      </c>
+      <c r="B85" s="4"/>
+    </row>
+    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="4" t="n">
+        <v>39385</v>
+      </c>
+      <c r="B86" s="4" t="n">
+        <v>39386</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="4" t="n">
+        <v>39343</v>
+      </c>
+      <c r="B87" s="4"/>
+    </row>
+    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="4" t="n">
+        <v>39301</v>
+      </c>
+      <c r="B88" s="4"/>
+    </row>
+    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="4" t="n">
+        <v>39260</v>
+      </c>
+      <c r="B89" s="4" t="n">
+        <v>39261</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="4" t="n">
+        <v>39211</v>
+      </c>
+      <c r="B90" s="4"/>
+    </row>
+    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="4" t="n">
+        <v>39161</v>
+      </c>
+      <c r="B91" s="4" t="n">
+        <v>39162</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="4" t="n">
+        <v>39112</v>
+      </c>
+      <c r="B92" s="4" t="n">
+        <v>39113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>